<commit_message>
Se juntan la ingesta, excel y la auditoria en un mismo archivo ingesta.py
</commit_message>
<xml_diff>
--- a/src/bigdata/static/xlsx/export_books.xlsx
+++ b/src/bigdata/static/xlsx/export_books.xlsx
@@ -571,54 +571,54 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>EqA6DwAAQBAJ</t>
+          <t>AGBCEAAAQBAJ</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Juego de tronos y la filosofía</t>
+          <t>Juego de tronos. Realidades, ficciones, turismos</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>La lógica es más afilada que las espadas. Se acerca la casa del dragón. Todo lo que siempre has querido saber sobre Juego de tronos, el maravilloso universo creado por R.R. Martin. ¿Son el honor y la verdad necesarios para conseguir la felicidad, o bien nos impiden llegar a ella? ¿Pueden los huargos y otras criaturas fantásticas revelarnos las verdades sobre nuestra conciencia y nuestra realidad? ¿La profecía nos demuestra que somos meros peones del destino o bien que somos libres de vivir una vida auténtica? Si las series de televisión son ideales para el análisis filosófico, Juego de tronos lo es por partida doble. En Westeros y más allá del Mar Angosto, el mundo de George R.R. Martin está repleto de docenas de personajes complejos en conflicto con ellos mismos y en lucha con otros, dudando de sí mismos, abocados al riesgo moral, al engaño, a la incertidumbre, a la arrogancia y a la agitación social y política. Mientras los Siete Reinos están en guerra, más allá del Muro, los horrores del invierno se acercan. Muy lejos, una joven reina lucha con su destino mientras viaja para recuperar su hogar. Todo esto es sabido, pero esta guía perspicaz se basa en las obras de Maquiavelo, Hobbes, Descartes, San Agustín, Platón, Aristóteles y muchos otros grandes filósofos para analizar los personajes y argumentos clave, mientras explora temas como la guerra, el honor, el conocimiento, la moral, la teoría de género y mucho más de una manera tan amena como sorprendente. La crítica ha dicho... «Aplica las teorías de filósofos como Platón, Aristóteles, Kant o Hume para intentar dar explicación a las motivaciones y los conflictos de los personajes de "Juego de tronos". Y que permite a su vez que los lectores se acerquen de una forma curiosa y divertida a esa área del conocimiento humano que es la filosofía.» Fantasymundo «Puede ser la luz que necesitamos para ver y comprender mejor la historia.» The Perks of Being More than a Reader «Sumamente disfrutable.» El Economista «Analiza algunos de los temas claves de la historia de Martin a la luz de los grandes pensadores: honor guerra, conocimiento, moral, verdad...» El norte de Castilla «Me he dado cuenta de muchas cosas de la historia, del porqué de muchos actos de variospersonajes, el arco de unos, las razones de algunas muertes, etc. De pararte a reflexionar con cada línea.» ABIBLIOPHOBICX</t>
+          <t>La influencia de los rodajes cinematográficos o televisivos en el interés turístico de determinados destinos ha ido tomando fuerza en los últimos años. En este libro analizamos el caso del rodaje de una superproducción internacional como es Juego de tronos en localizaciones de Irlanda del Norte o Girona, entre otras, examinando su repercusión en clave turística y los modos en que se entrelazan los atractivos preexistentes con la ficción creada por la productora HBO a partir de los libros de George R. R. Martin. Desde la especificidad del uso turístico de una de las series más exitosas de los últimos años podemos extrapolar diferentes reflexiones relacionadas con fenómenos como la construcción de cánones culturales i de imaginarios, o la noción de autoría en una contemporaneidad en la cual las expectativas del público ganan terreno.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2018-01-18</t>
+          <t>2021-09-10</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Henry Jacoby, William Irwin</t>
+          <t>Pere Parramon, F. Xavier Medina</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>N12OngEACAAJ</t>
+          <t>EqA6DwAAQBAJ</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Game of Thrones</t>
+          <t>Juego de tronos y la filosofía</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Inspired by the Emmy® Award–winning credits sequence that opens each episode of the hit HBO® series, Game of Thrones: A Pop-Up Guide to Westeros is guaranteed to thrill the show’s legions of fans. Featuring stunning pop-up recreations of several key locations from the series, including the formidable castle of Winterfell, the lavish capital city King’s Landing, and the Wall’s stark majesty, this book—designed by renowned paper engineer Matthew Reinhart—takes you into the world of the series like never before. Game of Thrones: A Pop-Up Guide to Westeros features a total of five stunning spreads, which fold out to create a remarkable pop-up map of Westeros that is perfect for displaying. The book also contains numerous mini-pops that bring to life iconic elements of the show, such as direwolves, White Walkers, giants, and dragons. All the pops are accompanied by insightful text that relays the rich history of the Seven Kingdoms and beyond, forming a dynamic reference guide to the world of Game of Thrones. Visually spectacular and enthrallingly interactive, Game of Thrones: A Pop-Up Guide to Westeros sets a new standard for pop-up books and perfectly captures the epic scope and imagination of the series.</t>
+          <t>La lógica es más afilada que las espadas. Se acerca la casa del dragón. Todo lo que siempre has querido saber sobre Juego de tronos, el maravilloso universo creado por R.R. Martin. ¿Son el honor y la verdad necesarios para conseguir la felicidad, o bien nos impiden llegar a ella? ¿Pueden los huargos y otras criaturas fantásticas revelarnos las verdades sobre nuestra conciencia y nuestra realidad? ¿La profecía nos demuestra que somos meros peones del destino o bien que somos libres de vivir una vida auténtica? Si las series de televisión son ideales para el análisis filosófico, Juego de tronos lo es por partida doble. En Westeros y más allá del Mar Angosto, el mundo de George R.R. Martin está repleto de docenas de personajes complejos en conflicto con ellos mismos y en lucha con otros, dudando de sí mismos, abocados al riesgo moral, al engaño, a la incertidumbre, a la arrogancia y a la agitación social y política. Mientras los Siete Reinos están en guerra, más allá del Muro, los horrores del invierno se acercan. Muy lejos, una joven reina lucha con su destino mientras viaja para recuperar su hogar. Todo esto es sabido, pero esta guía perspicaz se basa en las obras de Maquiavelo, Hobbes, Descartes, San Agustín, Platón, Aristóteles y muchos otros grandes filósofos para analizar los personajes y argumentos clave, mientras explora temas como la guerra, el honor, el conocimiento, la moral, la teoría de género y mucho más de una manera tan amena como sorprendente. La crítica ha dicho... «Aplica las teorías de filósofos como Platón, Aristóteles, Kant o Hume para intentar dar explicación a las motivaciones y los conflictos de los personajes de "Juego de tronos". Y que permite a su vez que los lectores se acerquen de una forma curiosa y divertida a esa área del conocimiento humano que es la filosofía.» Fantasymundo «Puede ser la luz que necesitamos para ver y comprender mejor la historia.» The Perks of Being More than a Reader «Sumamente disfrutable.» El Economista «Analiza algunos de los temas claves de la historia de Martin a la luz de los grandes pensadores: honor guerra, conocimiento, moral, verdad...» El norte de Castilla «Me he dado cuenta de muchas cosas de la historia, del porqué de muchos actos de variospersonajes, el arco de unos, las razones de algunas muertes, etc. De pararte a reflexionar con cada línea.» ABIBLIOPHOBICX</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2014-06-10</t>
+          <t>2018-01-18</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Matthew Reinhart</t>
+          <t>Henry Jacoby, William Irwin</t>
         </is>
       </c>
     </row>
@@ -679,54 +679,54 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>vfdIEAAAQBAJ</t>
+          <t>sbPj0AEACAAJ</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Juego de tronos. Realidades, ficciones, turismos</t>
+          <t>Juego de tronos</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>La influencia de los rodajes cinematográficos o televisivos en el interés turístico de determinados destinos ha ido tomando fuerza en los últimos años. En este libro analizamos el caso del rodaje de una superproducción internacional como es Juego de tronos en localizaciones de Irlanda del Norte o Girona, entre otras, examinando su repercusión en clave turística y los modos en que se entrelazan los atractivos preexistentes con la ficción creada por la productora HBO a partir de los libros de George R. R. Martin. Desde la especificidad del uso turístico de una de las series más exitosas de los últimos años podemos extrapolar diferentes reflexiones relacionadas con fenómenos como la construcción de cánones culturales y de imaginarios, o la noción de autoría en una contemporaneidad en la cual las expectativas del público ganan terreno.</t>
+          <t>Desconocido</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2021-10-11</t>
+          <t>2018</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Pere Parramon Rubio, Francesc Xavier Medina Luque</t>
+          <t>George R.R Martin</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>zL5VdKN76gEC</t>
+          <t>vfdIEAAAQBAJ</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>The Complete Sherlock Holmes</t>
+          <t>Juego de tronos. Realidades, ficciones, turismos</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Presents the four novels and fifty-six short stories which comprise the entire Sherlock Holmes saga</t>
+          <t>La influencia de los rodajes cinematográficos o televisivos en el interés turístico de determinados destinos ha ido tomando fuerza en los últimos años. En este libro analizamos el caso del rodaje de una superproducción internacional como es Juego de tronos en localizaciones de Irlanda del Norte o Girona, entre otras, examinando su repercusión en clave turística y los modos en que se entrelazan los atractivos preexistentes con la ficción creada por la productora HBO a partir de los libros de George R. R. Martin. Desde la especificidad del uso turístico de una de las series más exitosas de los últimos años podemos extrapolar diferentes reflexiones relacionadas con fenómenos como la construcción de cánones culturales y de imaginarios, o la noción de autoría en una contemporaneidad en la cual las expectativas del público ganan terreno.</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1930</t>
+          <t>2021-10-11</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Arthur Conan Doyle, Sir Arthur Conan Doyle</t>
+          <t>Pere Parramon Rubio, Francesc Xavier Medina Luque</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Generacion informe prueba json
</commit_message>
<xml_diff>
--- a/src/bigdata/static/xlsx/export_books.xlsx
+++ b/src/bigdata/static/xlsx/export_books.xlsx
@@ -571,54 +571,54 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>AGBCEAAAQBAJ</t>
+          <t>EqA6DwAAQBAJ</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Juego de tronos. Realidades, ficciones, turismos</t>
+          <t>Juego de tronos y la filosofía</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>La influencia de los rodajes cinematográficos o televisivos en el interés turístico de determinados destinos ha ido tomando fuerza en los últimos años. En este libro analizamos el caso del rodaje de una superproducción internacional como es Juego de tronos en localizaciones de Irlanda del Norte o Girona, entre otras, examinando su repercusión en clave turística y los modos en que se entrelazan los atractivos preexistentes con la ficción creada por la productora HBO a partir de los libros de George R. R. Martin. Desde la especificidad del uso turístico de una de las series más exitosas de los últimos años podemos extrapolar diferentes reflexiones relacionadas con fenómenos como la construcción de cánones culturales i de imaginarios, o la noción de autoría en una contemporaneidad en la cual las expectativas del público ganan terreno.</t>
+          <t>La lógica es más afilada que las espadas. Se acerca la casa del dragón. Todo lo que siempre has querido saber sobre Juego de tronos, el maravilloso universo creado por R.R. Martin. ¿Son el honor y la verdad necesarios para conseguir la felicidad, o bien nos impiden llegar a ella? ¿Pueden los huargos y otras criaturas fantásticas revelarnos las verdades sobre nuestra conciencia y nuestra realidad? ¿La profecía nos demuestra que somos meros peones del destino o bien que somos libres de vivir una vida auténtica? Si las series de televisión son ideales para el análisis filosófico, Juego de tronos lo es por partida doble. En Westeros y más allá del Mar Angosto, el mundo de George R.R. Martin está repleto de docenas de personajes complejos en conflicto con ellos mismos y en lucha con otros, dudando de sí mismos, abocados al riesgo moral, al engaño, a la incertidumbre, a la arrogancia y a la agitación social y política. Mientras los Siete Reinos están en guerra, más allá del Muro, los horrores del invierno se acercan. Muy lejos, una joven reina lucha con su destino mientras viaja para recuperar su hogar. Todo esto es sabido, pero esta guía perspicaz se basa en las obras de Maquiavelo, Hobbes, Descartes, San Agustín, Platón, Aristóteles y muchos otros grandes filósofos para analizar los personajes y argumentos clave, mientras explora temas como la guerra, el honor, el conocimiento, la moral, la teoría de género y mucho más de una manera tan amena como sorprendente. La crítica ha dicho... «Aplica las teorías de filósofos como Platón, Aristóteles, Kant o Hume para intentar dar explicación a las motivaciones y los conflictos de los personajes de "Juego de tronos". Y que permite a su vez que los lectores se acerquen de una forma curiosa y divertida a esa área del conocimiento humano que es la filosofía.» Fantasymundo «Puede ser la luz que necesitamos para ver y comprender mejor la historia.» The Perks of Being More than a Reader «Sumamente disfrutable.» El Economista «Analiza algunos de los temas claves de la historia de Martin a la luz de los grandes pensadores: honor guerra, conocimiento, moral, verdad...» El norte de Castilla «Me he dado cuenta de muchas cosas de la historia, del porqué de muchos actos de variospersonajes, el arco de unos, las razones de algunas muertes, etc. De pararte a reflexionar con cada línea.» ABIBLIOPHOBICX</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2021-09-10</t>
+          <t>2018-01-18</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Pere Parramon, F. Xavier Medina</t>
+          <t>Henry Jacoby, William Irwin</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>EqA6DwAAQBAJ</t>
+          <t>N12OngEACAAJ</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Juego de tronos y la filosofía</t>
+          <t>Game of Thrones</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>La lógica es más afilada que las espadas. Se acerca la casa del dragón. Todo lo que siempre has querido saber sobre Juego de tronos, el maravilloso universo creado por R.R. Martin. ¿Son el honor y la verdad necesarios para conseguir la felicidad, o bien nos impiden llegar a ella? ¿Pueden los huargos y otras criaturas fantásticas revelarnos las verdades sobre nuestra conciencia y nuestra realidad? ¿La profecía nos demuestra que somos meros peones del destino o bien que somos libres de vivir una vida auténtica? Si las series de televisión son ideales para el análisis filosófico, Juego de tronos lo es por partida doble. En Westeros y más allá del Mar Angosto, el mundo de George R.R. Martin está repleto de docenas de personajes complejos en conflicto con ellos mismos y en lucha con otros, dudando de sí mismos, abocados al riesgo moral, al engaño, a la incertidumbre, a la arrogancia y a la agitación social y política. Mientras los Siete Reinos están en guerra, más allá del Muro, los horrores del invierno se acercan. Muy lejos, una joven reina lucha con su destino mientras viaja para recuperar su hogar. Todo esto es sabido, pero esta guía perspicaz se basa en las obras de Maquiavelo, Hobbes, Descartes, San Agustín, Platón, Aristóteles y muchos otros grandes filósofos para analizar los personajes y argumentos clave, mientras explora temas como la guerra, el honor, el conocimiento, la moral, la teoría de género y mucho más de una manera tan amena como sorprendente. La crítica ha dicho... «Aplica las teorías de filósofos como Platón, Aristóteles, Kant o Hume para intentar dar explicación a las motivaciones y los conflictos de los personajes de "Juego de tronos". Y que permite a su vez que los lectores se acerquen de una forma curiosa y divertida a esa área del conocimiento humano que es la filosofía.» Fantasymundo «Puede ser la luz que necesitamos para ver y comprender mejor la historia.» The Perks of Being More than a Reader «Sumamente disfrutable.» El Economista «Analiza algunos de los temas claves de la historia de Martin a la luz de los grandes pensadores: honor guerra, conocimiento, moral, verdad...» El norte de Castilla «Me he dado cuenta de muchas cosas de la historia, del porqué de muchos actos de variospersonajes, el arco de unos, las razones de algunas muertes, etc. De pararte a reflexionar con cada línea.» ABIBLIOPHOBICX</t>
+          <t>Inspired by the Emmy® Award–winning credits sequence that opens each episode of the hit HBO® series, Game of Thrones: A Pop-Up Guide to Westeros is guaranteed to thrill the show’s legions of fans. Featuring stunning pop-up recreations of several key locations from the series, including the formidable castle of Winterfell, the lavish capital city King’s Landing, and the Wall’s stark majesty, this book—designed by renowned paper engineer Matthew Reinhart—takes you into the world of the series like never before. Game of Thrones: A Pop-Up Guide to Westeros features a total of five stunning spreads, which fold out to create a remarkable pop-up map of Westeros that is perfect for displaying. The book also contains numerous mini-pops that bring to life iconic elements of the show, such as direwolves, White Walkers, giants, and dragons. All the pops are accompanied by insightful text that relays the rich history of the Seven Kingdoms and beyond, forming a dynamic reference guide to the world of Game of Thrones. Visually spectacular and enthrallingly interactive, Game of Thrones: A Pop-Up Guide to Westeros sets a new standard for pop-up books and perfectly captures the epic scope and imagination of the series.</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2018-01-18</t>
+          <t>2014-06-10</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Henry Jacoby, William Irwin</t>
+          <t>Matthew Reinhart</t>
         </is>
       </c>
     </row>
@@ -679,54 +679,54 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>sbPj0AEACAAJ</t>
+          <t>vfdIEAAAQBAJ</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Juego de tronos</t>
+          <t>Juego de tronos. Realidades, ficciones, turismos</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>La influencia de los rodajes cinematográficos o televisivos en el interés turístico de determinados destinos ha ido tomando fuerza en los últimos años. En este libro analizamos el caso del rodaje de una superproducción internacional como es Juego de tronos en localizaciones de Irlanda del Norte o Girona, entre otras, examinando su repercusión en clave turística y los modos en que se entrelazan los atractivos preexistentes con la ficción creada por la productora HBO a partir de los libros de George R. R. Martin. Desde la especificidad del uso turístico de una de las series más exitosas de los últimos años podemos extrapolar diferentes reflexiones relacionadas con fenómenos como la construcción de cánones culturales y de imaginarios, o la noción de autoría en una contemporaneidad en la cual las expectativas del público ganan terreno.</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2018</t>
+          <t>2021-10-11</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>George R.R Martin</t>
+          <t>Pere Parramon Rubio, Francesc Xavier Medina Luque</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>vfdIEAAAQBAJ</t>
+          <t>zL5VdKN76gEC</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Juego de tronos. Realidades, ficciones, turismos</t>
+          <t>The Complete Sherlock Holmes</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>La influencia de los rodajes cinematográficos o televisivos en el interés turístico de determinados destinos ha ido tomando fuerza en los últimos años. En este libro analizamos el caso del rodaje de una superproducción internacional como es Juego de tronos en localizaciones de Irlanda del Norte o Girona, entre otras, examinando su repercusión en clave turística y los modos en que se entrelazan los atractivos preexistentes con la ficción creada por la productora HBO a partir de los libros de George R. R. Martin. Desde la especificidad del uso turístico de una de las series más exitosas de los últimos años podemos extrapolar diferentes reflexiones relacionadas con fenómenos como la construcción de cánones culturales y de imaginarios, o la noción de autoría en una contemporaneidad en la cual las expectativas del público ganan terreno.</t>
+          <t>Presents the four novels and fifty-six short stories which comprise the entire Sherlock Holmes saga</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2021-10-11</t>
+          <t>1930</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Pere Parramon Rubio, Francesc Xavier Medina Luque</t>
+          <t>Arthur Conan Doyle, Sir Arthur Conan Doyle</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Auditoria limpieza sin codigo comentado.
</commit_message>
<xml_diff>
--- a/src/bigdata/static/xlsx/export_books.xlsx
+++ b/src/bigdata/static/xlsx/export_books.xlsx
@@ -517,81 +517,81 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>6sRGzwEACAAJ</t>
+          <t>Av6RMQEACAAJ</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>El Señor de Los Anillos. La Comunidad Del Anillo (TV Tie-In) (the Lord of the Rings. the Fellowship of the Ring [Tv Tie-In]) (Spanish Edition)</t>
+          <t>La comunidad del anillo</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Un héroe inesperado. Una misión peligrosa. La mayor aventura que jamás te hayan contado. La primera entrega de la trilogía de J. R. R. Tolkien El Señor de los Anillos En la adormecida e idílica Comarca, un joven hobbit recibe un encargo: custodiar el Anillo Único y emprender el viaje para su destrucción en la Grieta del Destino. Acompañado por magos, hombres, elfos y enanos, atravesará la Tierra Media y se internará en las sombras de Mordor, perseguido siempre por las huestes de Sauron, el Señor Oscuro, dispuesto a recuperar su creación para establecer el dominio definitivo del Mal. «La obra de Tolkien, difundida en millones de ejemplares, traducida a docenas de lenguas, inspiradora de slogans pintados en las paredes de Nueva York y de Buenos Aires... una coherente mitología de una autenticidad universal creada en pleno siglo veinte.» --George Steiner, Le Monde, 1973 ENGLISH DESCRIPTION Inspired by The Hobbit and begun in 1937, The Lord of the Rings is a trilogy that J.R.R. Tolkien created to provide "the necessary background of history for Elvish tongues". From these academic aspirations was born one of the most popular and imaginative works in English literature. The Fellowship of the Ring, the first volume in the trilogy, tells of the fateful power of the One Ring. It begins a magnificent tale of adventure that will plunge the members of the Fellowship of the Ring into a perilous quest and set the stage for the ultimate clash between the powers of good and evil. In this splendid, unabridged audio production of Tolkien's great work, all the inhabitants of a magical universe - hobbits, elves, and wizards - step colorfully into life. Rob Inglis' narration has been praised as a masterpiece of audio.</t>
+          <t>En la adormecida e idilica Comarca, un joven hobbit recibe un encargo : custodiar el Anillo Único y emprender el viaje para su destrucción en las Grietas del Destino. Acompañado por magos, hombres, elfos y enanos, atravesará la Tierra Media y se internará en las sombras de Mordor, perseguido siempre por las huestes de Sauron, el Señor Oscuro, dispuesto a recuperar su creación para establecer el dominio definitivo del Mal. (Source : 4e de couverture).</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2022-09-27</t>
+          <t>2012</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>J. R. R. Tolkien</t>
+          <t>John Ronald Reuel Tolkien</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Av6RMQEACAAJ</t>
+          <t>DYmUGGwZ8_oC</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>La comunidad del anillo</t>
+          <t>El Señor de los Anillos no 01/03 La Comunidad del Anillo (edición revisada)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>En la adormecida e idilica Comarca, un joven hobbit recibe un encargo : custodiar el Anillo Único y emprender el viaje para su destrucción en las Grietas del Destino. Acompañado por magos, hombres, elfos y enanos, atravesará la Tierra Media y se internará en las sombras de Mordor, perseguido siempre por las huestes de Sauron, el Señor Oscuro, dispuesto a recuperar su creación para establecer el dominio definitivo del Mal. (Source : 4e de couverture).</t>
+          <t>Primera entrega de la trilogía. «Este libro es como un relámpago en un cielo claro. Decir que la novela heroica, espléndida, elocuente y desinhibida, ha retornado de pronto en una época de un antirromanticismo casi patológico, sería inadecuado. Para quienes vivimos en esa extraña época, el retorno —y el alivio que nos trae— es sin duda lo más importante. Pero para la historia misma de la novela —una historia que se remonta a la Odisea y a antes de la Odisea— no es un retorno, sino un paso adelante o una revolución: la conquista de un territorio nuevo.» —C.S. Lewis, Time &amp; Tide, 1954 «La obra de Tolkien, difundida en millones de ejemplares, traducida a docenas de lenguas, inspiradora de slogans pintados en las paredes de Nueva York y de Buenos Aires... una coherente mitología de una autenticidad universal creada en pleno siglo veinte.» —George Steiner, Le Monde, 1973</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2012</t>
+          <t>2010-07-15</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>John Ronald Reuel Tolkien</t>
+          <t>J. R. R. Tolkien</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>DYmUGGwZ8_oC</t>
+          <t>FlGcUAnpMmIC</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>El Señor de los Anillos no 01/03 La Comunidad del Anillo (edición revisada)</t>
+          <t>Hobbit's Travels</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Primera entrega de la trilogía. «Este libro es como un relámpago en un cielo claro. Decir que la novela heroica, espléndida, elocuente y desinhibida, ha retornado de pronto en una época de un antirromanticismo casi patológico, sería inadecuado. Para quienes vivimos en esa extraña época, el retorno —y el alivio que nos trae— es sin duda lo más importante. Pero para la historia misma de la novela —una historia que se remonta a la Odisea y a antes de la Odisea— no es un retorno, sino un paso adelante o una revolución: la conquista de un territorio nuevo.» —C.S. Lewis, Time &amp; Tide, 1954 «La obra de Tolkien, difundida en millones de ejemplares, traducida a docenas de lenguas, inspiradora de slogans pintados en las paredes de Nueva York y de Buenos Aires... una coherente mitología de una autenticidad universal creada en pleno siglo veinte.» —George Steiner, Le Monde, 1973</t>
+          <t>Printed on deluxe recycled parchment paper, this journal celebrating J. R. R. Tolkien's classic tales makes a lovely gift, and is just as nice to keep! With magical two-color illustrations throughout (drawings made by Frodo Baggins's devoted companion, Sam Gamgee, on their travels throughout Middle-earth), it provides ample space for recording personal thoughts, reflections on Tolkien's masterpiece, or fantasies of your own creation.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2010-07-15</t>
+          <t>2002-01-04</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>J. R. R. Tolkien</t>
+          <t>Sam Gamgee</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
limpieza auditoria en main.
</commit_message>
<xml_diff>
--- a/src/bigdata/static/xlsx/export_books.xlsx
+++ b/src/bigdata/static/xlsx/export_books.xlsx
@@ -652,88 +652,88 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>JUdOAAAACAAJ</t>
+          <t>LCZvVRqH-m8C</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>The Lord of the Rings Sketchbook</t>
+          <t>El señor de los anillos</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>"In The Lord of the Rings Sketchbook Alan Lee reveals in pictures and in words how he created the watercolor paintings for the special centenary edition of The Lord of the Rings. These images would prove so powerful and evocative that they would eventually define the look of Peter Jackson's movie trilogy and earn him a coveted Academy Award." "The book is filled with more than 150 of his sketches and early conceptual pieces showing how the project progressed from idea to finished art. It also contains a selection of full-page paintings reproduced in full color, together with numerous examples of previously unseen conceptual art produced for the films and many new works drawn specially for this book." "The Lord of the Rings Sketchbook provides an insight into the imagination of the man who painted Tolkien's vision, first on the page and then in three dimensions on the movie screen. It will also be of interest to many of the thousands of people who have bought the illustrated Lord of the Rings as well as to budding artists who want to unlock the secrets of book illustration."--BOOK JACKET.</t>
+          <t>Desconocido</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2005</t>
+          <t>1999-05</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Alan Lee</t>
+          <t>Terry Donaldson</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>LCZvVRqH-m8C</t>
+          <t>LvsQ34A1fOMC</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>El señor de los anillos</t>
+          <t>El Señor de los Anillos no 03/03 El Retorno del Rey (edición revisada)</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>La tercera entrega de la trilogía El Señor de los Anillos. Los ejércitos del Señor Oscuro van extendiendo cada vez más su maléfica sombra por la Tierra Media. Hombres, elfos y enanos unen sus fuerzas para presentar batalla a Sauron y sus huestes. Ajenos a estos preparativos, Frodo y Sam siguen adentrándose en el país de Mordor en su heroico viaje para destruir el Anillo de Poder en las Grietas del Destino. «Un final triunfante... un gran trabajo, tanto en la concepción como en la ejecución.» —Daily Telegraph «Un trabajo extraordinariamente imaginativo, parte saga, parte alegoría, y emocionante en su totalidad.» —The Times</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1999-05</t>
+          <t>2010-07-15</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Terry Donaldson</t>
+          <t>J. R. R. Tolkien</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>LvsQ34A1fOMC</t>
+          <t>Ndgf0AEACAAJ</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>El Señor de los Anillos no 03/03 El Retorno del Rey (edición revisada)</t>
+          <t>El señor de los anillos</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>La tercera entrega de la trilogía El Señor de los Anillos. Los ejércitos del Señor Oscuro van extendiendo cada vez más su maléfica sombra por la Tierra Media. Hombres, elfos y enanos unen sus fuerzas para presentar batalla a Sauron y sus huestes. Ajenos a estos preparativos, Frodo y Sam siguen adentrándose en el país de Mordor en su heroico viaje para destruir el Anillo de Poder en las Grietas del Destino. «Un final triunfante... un gran trabajo, tanto en la concepción como en la ejecución.» —Daily Telegraph «Un trabajo extraordinariamente imaginativo, parte saga, parte alegoría, y emocionante en su totalidad.» —The Times</t>
+          <t>Desconocido</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2010-07-15</t>
+          <t>2007</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>J. R. R. Tolkien</t>
+          <t>John Ronald Reuel Tolkien</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Ndgf0AEACAAJ</t>
+          <t>QtSEvgEACAAJ</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -748,7 +748,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2007</t>
+          <t>1998</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -760,12 +760,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>QtSEvgEACAAJ</t>
+          <t>RYr8sgEACAAJ</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>El señor de los anillos</t>
+          <t>Fellowship of the Ring</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -775,24 +775,20 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>1998</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>John Ronald Reuel Tolkien</t>
-        </is>
-      </c>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>RYr8sgEACAAJ</t>
+          <t>T8P3AAAACAAJ</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Fellowship of the Ring</t>
+          <t>Tolkien, el Señor de Los Anillos</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -802,74 +798,74 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2000</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr"/>
+          <t>2004-09-01</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>J. R. R. Tolkien</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>T8P3AAAACAAJ</t>
+          <t>U7sA0AEACAAJ</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Tolkien, el Señor de Los Anillos</t>
+          <t>El Señor de los Anillos III</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>Los ejércitos del Señor Oscuro van extendiendo cada vez más su maléfica sombra por la Tierra Media. Hombres, elfos y enanos unen sus fuerzas para presentar batalla a Sauron y sus huestes. Ajenos a estos preparativos, Frodo y Sam siguen adentrándose en el país de Mordor en su heroico viaje para destruir el Anillo de Poder en las Grietas del Destino.</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2004-09-01</t>
+          <t>2010-04-28</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>J. R. R. Tolkien</t>
+          <t>John Ronald Reuel Tolkien</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>U7sA0AEACAAJ</t>
+          <t>WBOxAQAACAAJ</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>El Señor de los Anillos III</t>
+          <t>El Senor de Los Anillos</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Los ejércitos del Señor Oscuro van extendiendo cada vez más su maléfica sombra por la Tierra Media. Hombres, elfos y enanos unen sus fuerzas para presentar batalla a Sauron y sus huestes. Ajenos a estos preparativos, Frodo y Sam siguen adentrándose en el país de Mordor en su heroico viaje para destruir el Anillo de Poder en las Grietas del Destino.</t>
+          <t>Desconocido</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2010-04-28</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>John Ronald Reuel Tolkien</t>
-        </is>
-      </c>
+          <t>2007</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>WBOxAQAACAAJ</t>
+          <t>WmdWtQAACAAJ</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>El Senor de Los Anillos</t>
+          <t>El Señor de los anillos</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -879,20 +875,24 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2007</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr"/>
+          <t>2002</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>J. R. R. Tolkien</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>WmdWtQAACAAJ</t>
+          <t>ZVwX0QEACAAJ</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>El Señor de los anillos</t>
+          <t>El Señor de los Anillos</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -902,7 +902,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2002</t>
+          <t>1985</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -914,12 +914,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>ZVwX0QEACAAJ</t>
+          <t>ayczzwEACAAJ</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>El Señor de los Anillos</t>
+          <t>El señor de los anillos</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -929,19 +929,19 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1985</t>
+          <t>1988</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>J. R. R. Tolkien</t>
+          <t>John Ronald Ruelen Tolkien</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>ayczzwEACAAJ</t>
+          <t>cURzPgAACAAJ</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -956,61 +956,61 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1988</t>
+          <t>1993</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>John Ronald Ruelen Tolkien</t>
+          <t>John Ronald Reuel Tolkien</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>cURzPgAACAAJ</t>
+          <t>e1ZJzwEACAAJ</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>El señor de los anillos</t>
+          <t>El Señor de Los Anillos 3. El Retorno del Rey (TV Tie-In). the Lord of the Rings 3. the Return of the King (TV Tie-In) (Spanish Edition)</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>La última parte del viaje de Frodo y Sam Los ejércitos del Señor Oscuro van extendiendo cada vez más su maléfica sombra por la Tierra Media. Hombres, elfos y enanos unen sus fuerzas para presentar batalla a Sauron y sus huestes. Ajenos a estos preparativos, Frodo y Sam siguen adentrándose en el país de Mordor en su heroico viaje para destruir el Anillo de Poder en las Grietas del Destino. ENGLISH DESCRIPTION The Return of the King is the third part of J.R.R. Tolkien's epic adventure The Lord of the Rings. One Ring to rule them all, One Ring to find them, One Ring to bring them all and in the darkness bind them. The Dark Lord has risen, and as he unleashes hordes of Orcs to conquer all Middle-earth, Frodo and Sam struggle deep into his realm in Mordor. To defeat Sauron, the One Ring must be destroyed in the fires of Mount Doom. But the way is impossibly hard, and Frodo is weakening. The Ring corrupts all who bear it and Frodo's time is running out. Will Sam and Frodo succeed, or will the Dark Lord rule Middle-earth once more?</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1993</t>
+          <t>2022-09-27</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>John Ronald Reuel Tolkien</t>
+          <t>J. R. R. Tolkien</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>e1ZJzwEACAAJ</t>
+          <t>eqPUjwEACAAJ</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>El Señor de Los Anillos 3. El Retorno del Rey (TV Tie-In). the Lord of the Rings 3. the Return of the King (TV Tie-In) (Spanish Edition)</t>
+          <t>El Senor de Los Anillos</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>La última parte del viaje de Frodo y Sam Los ejércitos del Señor Oscuro van extendiendo cada vez más su maléfica sombra por la Tierra Media. Hombres, elfos y enanos unen sus fuerzas para presentar batalla a Sauron y sus huestes. Ajenos a estos preparativos, Frodo y Sam siguen adentrándose en el país de Mordor en su heroico viaje para destruir el Anillo de Poder en las Grietas del Destino. ENGLISH DESCRIPTION The Return of the King is the third part of J.R.R. Tolkien's epic adventure The Lord of the Rings. One Ring to rule them all, One Ring to find them, One Ring to bring them all and in the darkness bind them. The Dark Lord has risen, and as he unleashes hordes of Orcs to conquer all Middle-earth, Frodo and Sam struggle deep into his realm in Mordor. To defeat Sauron, the One Ring must be destroyed in the fires of Mount Doom. But the way is impossibly hard, and Frodo is weakening. The Ring corrupts all who bear it and Frodo's time is running out. Will Sam and Frodo succeed, or will the Dark Lord rule Middle-earth once more?</t>
+          <t>Titulo: El Señor de los anillos: La comunidad del anillo.Autor: J. R. R. Tolkien.Fecha de publicación: 1954.En la adormecida e idílica Comarca, un joven hobbit recibe un encargo: custodiar el Anillo Único y emprender el viaje para su destrucción en las Grietas del Destino. Acompañado por magos, hombres, elfos y enanos, atravesará la Tierra Media y se internará en las sombras de Mordor, perseguido siempre por las huestes de Sauron, el Señor Oscuro, dispuesto a recuperar su creación para establecer el dominio definitivo del Mal.</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2022-09-27</t>
+          <t>2016-05-31</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">

</xml_diff>

<commit_message>
Generación de informe de transformaciones
</commit_message>
<xml_diff>
--- a/src/bigdata/static/xlsx/export_books.xlsx
+++ b/src/bigdata/static/xlsx/export_books.xlsx
@@ -864,39 +864,39 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>U7sA0AEACAAJ</t>
+          <t>UfYGAAAACAAJ</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>El Señor de los Anillos III</t>
+          <t>El señor de los anillos</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Los ejércitos del Señor Oscuro van extendiendo cada vez más su maléfica sombra por la Tierra Media. Hombres, elfos y enanos unen sus fuerzas para presentar batalla a Sauron y sus huestes. Ajenos a estos preparativos, Frodo y Sam siguen adentrándose en el país de Mordor en su heroico viaje para destruir el Anillo de Poder en las Grietas del Destino.</t>
+          <t>Desconocido</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2010-04-28</t>
+          <t>2002-02</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>John Ronald Reuel Tolkien</t>
+          <t>Kurt D. Bruner, Jim Ware</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>UfYGAAAACAAJ</t>
+          <t>WmdWtQAACAAJ</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>El señor de los anillos</t>
+          <t>El Señor de los anillos</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -906,24 +906,24 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2002-02</t>
+          <t>2002</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Kurt D. Bruner, Jim Ware</t>
+          <t>J. R. R. Tolkien</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>WmdWtQAACAAJ</t>
+          <t>ZVwX0QEACAAJ</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>El Señor de los anillos</t>
+          <t>El Señor de los Anillos</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -933,7 +933,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2002</t>
+          <t>1985</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -945,22 +945,22 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>ZVwX0QEACAAJ</t>
+          <t>ZcAlEAAAQBAJ</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>El Señor de los Anillos</t>
+          <t>The Lord of the Rings Illustrated</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>A sumptuous slipcased edition of Tolkien's classic epic tale of adventure, fully illustrated in color by the author himself. This deluxe volume is quarterbound in leather and includes many special features unique to this edition. Since it was first published in 1954, The Lord of the Rings has been a book people have treasured. Steeped in unrivalled magic and otherworldliness, its sweeping fantasy and epic adventure has touched the hearts of young and old alike. Over 100 million copies of its many editions have been sold around the world, and occasional collectors' editions become prized and valuable items of publishing. This one-volume deluxe slipcased edition contains the complete text, fully corrected and reset, which is printed in red and black, and features thirty color illustrations, maps, and sketches drawn by Tolkien himself as he composed this epic work. These include the pages from the Book of Mazarbul, marvelous facsimiles created by Tolkien to accompany the famous "Bridge of Khazad-dum" chapter. Also appearing are two poster-size, fold-out maps revealing all the detail of Middle-earth. This very special deluxe edition is quarterbound in cloth and red leather, with raised ribs on the spine and stamped in two foils. The pages are edged in gold and contained within are special features unique to this edition.</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1985</t>
+          <t>2021-10-19</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">

</xml_diff>

<commit_message>
refinado de auditoria de transformacion.py final.
</commit_message>
<xml_diff>
--- a/src/bigdata/static/xlsx/export_books.xlsx
+++ b/src/bigdata/static/xlsx/export_books.xlsx
@@ -864,39 +864,39 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>U7sA0AEACAAJ</t>
+          <t>UfYGAAAACAAJ</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>El Señor de los Anillos III</t>
+          <t>El señor de los anillos</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Los ejércitos del Señor Oscuro van extendiendo cada vez más su maléfica sombra por la Tierra Media. Hombres, elfos y enanos unen sus fuerzas para presentar batalla a Sauron y sus huestes. Ajenos a estos preparativos, Frodo y Sam siguen adentrándose en el país de Mordor en su heroico viaje para destruir el Anillo de Poder en las Grietas del Destino.</t>
+          <t>Desconocido</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2010-04-28</t>
+          <t>2002-02</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>John Ronald Reuel Tolkien</t>
+          <t>Kurt D. Bruner, Jim Ware</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>UfYGAAAACAAJ</t>
+          <t>WmdWtQAACAAJ</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>El señor de los anillos</t>
+          <t>El Señor de los anillos</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -906,24 +906,24 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2002-02</t>
+          <t>2002</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Kurt D. Bruner, Jim Ware</t>
+          <t>J. R. R. Tolkien</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>WmdWtQAACAAJ</t>
+          <t>ZVwX0QEACAAJ</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>El Señor de los anillos</t>
+          <t>El Señor de los Anillos</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -933,7 +933,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2002</t>
+          <t>1985</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -945,22 +945,22 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>ZVwX0QEACAAJ</t>
+          <t>ZcAlEAAAQBAJ</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>El Señor de los Anillos</t>
+          <t>The Lord of the Rings Illustrated</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>A sumptuous slipcased edition of Tolkien's classic epic tale of adventure, fully illustrated in color by the author himself. This deluxe volume is quarterbound in leather and includes many special features unique to this edition. Since it was first published in 1954, The Lord of the Rings has been a book people have treasured. Steeped in unrivalled magic and otherworldliness, its sweeping fantasy and epic adventure has touched the hearts of young and old alike. Over 100 million copies of its many editions have been sold around the world, and occasional collectors' editions become prized and valuable items of publishing. This one-volume deluxe slipcased edition contains the complete text, fully corrected and reset, which is printed in red and black, and features thirty color illustrations, maps, and sketches drawn by Tolkien himself as he composed this epic work. These include the pages from the Book of Mazarbul, marvelous facsimiles created by Tolkien to accompany the famous "Bridge of Khazad-dum" chapter. Also appearing are two poster-size, fold-out maps revealing all the detail of Middle-earth. This very special deluxe edition is quarterbound in cloth and red leather, with raised ribs on the spine and stamped in two foils. The pages are edged in gold and contained within are special features unique to this edition.</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1985</t>
+          <t>2021-10-19</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">

</xml_diff>

<commit_message>
Autorizacion del profesor Callejas para cambio de auditoria de transformacion de texto a mostrar en terminal debido a run exitoso en codespace pero no en actions.
</commit_message>
<xml_diff>
--- a/src/bigdata/static/xlsx/export_books.xlsx
+++ b/src/bigdata/static/xlsx/export_books.xlsx
@@ -490,196 +490,196 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>6463zwEACAAJ</t>
+          <t>7abaCsl-b5MC</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>The return of the king</t>
+          <t>Tolkien</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>Pocos escritores vivos han conseguido atraer tanta atencion e interes, despertar tanta pasion y entusiasmo, suscitar tanta controversia y adulacion como J.R.R Tolkien. Curiosamente, nadie ha explorado los origenes de la obra cumbre de Tolkien, El Senor de los Anillos, ni ha intentado relacionarla con la larga saga de historias epicas en las que se inspira y de las que es, a la vez, ejemplo.El origen de El Senor de los Anillos es un ameno recorrido por las sagas heroicas, desde los mitos griegos hasta las mitologias nordicas, y los grandes relatos que, a traves del tiempo, se han convertido en la fuente e inspiracion de uno de los mayores narradores del siglo XX: J.R.R. Tolkien.El libro de Lin Carter constituye una lectura absorbente para los millones de seguidores de El Senor de los anillos y ofrece una fascinante introduccion para quienes deseen aproximarse por primera vez al universo magico de Tolkien.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1965</t>
+          <t>2002</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>John Ronald Reuel Tolkien</t>
+          <t>J. R. R. Tolkien, Lin Carter</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>7abaCsl-b5MC</t>
+          <t>DYmUGGwZ8_oC</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Tolkien</t>
+          <t>El Señor de los Anillos no 01/03 La Comunidad del Anillo (edición revisada)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Pocos escritores vivos han conseguido atraer tanta atencion e interes, despertar tanta pasion y entusiasmo, suscitar tanta controversia y adulacion como J.R.R Tolkien. Curiosamente, nadie ha explorado los origenes de la obra cumbre de Tolkien, El Senor de los Anillos, ni ha intentado relacionarla con la larga saga de historias epicas en las que se inspira y de las que es, a la vez, ejemplo.El origen de El Senor de los Anillos es un ameno recorrido por las sagas heroicas, desde los mitos griegos hasta las mitologias nordicas, y los grandes relatos que, a traves del tiempo, se han convertido en la fuente e inspiracion de uno de los mayores narradores del siglo XX: J.R.R. Tolkien.El libro de Lin Carter constituye una lectura absorbente para los millones de seguidores de El Senor de los anillos y ofrece una fascinante introduccion para quienes deseen aproximarse por primera vez al universo magico de Tolkien.</t>
+          <t>Primera entrega de la trilogía. «Este libro es como un relámpago en un cielo claro. Decir que la novela heroica, espléndida, elocuente y desinhibida, ha retornado de pronto en una época de un antirromanticismo casi patológico, sería inadecuado. Para quienes vivimos en esa extraña época, el retorno —y el alivio que nos trae— es sin duda lo más importante. Pero para la historia misma de la novela —una historia que se remonta a la Odisea y a antes de la Odisea— no es un retorno, sino un paso adelante o una revolución: la conquista de un territorio nuevo.» —C.S. Lewis, Time &amp; Tide, 1954 «La obra de Tolkien, difundida en millones de ejemplares, traducida a docenas de lenguas, inspiradora de slogans pintados en las paredes de Nueva York y de Buenos Aires... una coherente mitología de una autenticidad universal creada en pleno siglo veinte.» —George Steiner, Le Monde, 1973</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2002</t>
+          <t>2010-07-15</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>J. R. R. Tolkien, Lin Carter</t>
+          <t>J. R. R. Tolkien</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>DYmUGGwZ8_oC</t>
+          <t>GAcCAAAACAAJ</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>El Señor de los Anillos no 01/03 La Comunidad del Anillo (edición revisada)</t>
+          <t>Los mundos mágicos de El señor de los anillos</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Primera entrega de la trilogía. «Este libro es como un relámpago en un cielo claro. Decir que la novela heroica, espléndida, elocuente y desinhibida, ha retornado de pronto en una época de un antirromanticismo casi patológico, sería inadecuado. Para quienes vivimos en esa extraña época, el retorno —y el alivio que nos trae— es sin duda lo más importante. Pero para la historia misma de la novela —una historia que se remonta a la Odisea y a antes de la Odisea— no es un retorno, sino un paso adelante o una revolución: la conquista de un territorio nuevo.» —C.S. Lewis, Time &amp; Tide, 1954 «La obra de Tolkien, difundida en millones de ejemplares, traducida a docenas de lenguas, inspiradora de slogans pintados en las paredes de Nueva York y de Buenos Aires... una coherente mitología de una autenticidad universal creada en pleno siglo veinte.» —George Steiner, Le Monde, 1973</t>
+          <t>Desconocido</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2010-07-15</t>
+          <t>2003</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>J. R. R. Tolkien</t>
+          <t>David Colbert</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>GAcCAAAACAAJ</t>
+          <t>IOyjMQEACAAJ</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Los mundos mágicos de El señor de los anillos</t>
+          <t>The Power of the Ring</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>Digging deep into J. R. R. Tolkien's spiritual biography--his religious scholarship and his love of both Christian and pagan myth--Stratford Caldecott offers a critical study of how the acclaimed author effectively created a vivid Middle Earth using the familiar rites and ceremonies of human history. And while readers and moviegoers alike may appreciate the fantasy world of The Hobbit and the Lord of the Rings trilogy, few know that in life, Tolkien was a devout Roman Catholic and that the characters, the events, and the general morality of each novel are informed by the dogmas of his faith. Revised and updated, this acclaimed study of Tolkien's achievement--previously released as Secret Fire in the UK--includes commentary on Peter Jackson's film adaptations and explores many of the fascinating stories and letters published after Tolkien's death.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2003</t>
+          <t>2012-12-04</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>David Colbert</t>
+          <t>Stratford Caldecott</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Gdvd0AEACAAJ</t>
+          <t>JUdOAAAACAAJ</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>El señor de los anillos</t>
+          <t>The Lord of the Rings Sketchbook</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>"In The Lord of the Rings Sketchbook Alan Lee reveals in pictures and in words how he created the watercolor paintings for the special centenary edition of The Lord of the Rings. These images would prove so powerful and evocative that they would eventually define the look of Peter Jackson's movie trilogy and earn him a coveted Academy Award." "The book is filled with more than 150 of his sketches and early conceptual pieces showing how the project progressed from idea to finished art. It also contains a selection of full-page paintings reproduced in full color, together with numerous examples of previously unseen conceptual art produced for the films and many new works drawn specially for this book." "The Lord of the Rings Sketchbook provides an insight into the imagination of the man who painted Tolkien's vision, first on the page and then in three dimensions on the movie screen. It will also be of interest to many of the thousands of people who have bought the illustrated Lord of the Rings as well as to budding artists who want to unlock the secrets of book illustration."--BOOK JACKET.</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1993</t>
+          <t>2005</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>J. R. R. Tolkien</t>
+          <t>Alan Lee</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>IOyjMQEACAAJ</t>
+          <t>LCZvVRqH-m8C</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>The Power of the Ring</t>
+          <t>El señor de los anillos</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Digging deep into J. R. R. Tolkien's spiritual biography--his religious scholarship and his love of both Christian and pagan myth--Stratford Caldecott offers a critical study of how the acclaimed author effectively created a vivid Middle Earth using the familiar rites and ceremonies of human history. And while readers and moviegoers alike may appreciate the fantasy world of The Hobbit and the Lord of the Rings trilogy, few know that in life, Tolkien was a devout Roman Catholic and that the characters, the events, and the general morality of each novel are informed by the dogmas of his faith. Revised and updated, this acclaimed study of Tolkien's achievement--previously released as Secret Fire in the UK--includes commentary on Peter Jackson's film adaptations and explores many of the fascinating stories and letters published after Tolkien's death.</t>
+          <t>Desconocido</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2012-12-04</t>
+          <t>1999-05</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Stratford Caldecott</t>
+          <t>Terry Donaldson</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>JUdOAAAACAAJ</t>
+          <t>LvsQ34A1fOMC</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>The Lord of the Rings Sketchbook</t>
+          <t>El Señor de los Anillos no 03/03 El Retorno del Rey (edición revisada)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>"In The Lord of the Rings Sketchbook Alan Lee reveals in pictures and in words how he created the watercolor paintings for the special centenary edition of The Lord of the Rings. These images would prove so powerful and evocative that they would eventually define the look of Peter Jackson's movie trilogy and earn him a coveted Academy Award." "The book is filled with more than 150 of his sketches and early conceptual pieces showing how the project progressed from idea to finished art. It also contains a selection of full-page paintings reproduced in full color, together with numerous examples of previously unseen conceptual art produced for the films and many new works drawn specially for this book." "The Lord of the Rings Sketchbook provides an insight into the imagination of the man who painted Tolkien's vision, first on the page and then in three dimensions on the movie screen. It will also be of interest to many of the thousands of people who have bought the illustrated Lord of the Rings as well as to budding artists who want to unlock the secrets of book illustration."--BOOK JACKET.</t>
+          <t>La tercera entrega de la trilogía El Señor de los Anillos. Los ejércitos del Señor Oscuro van extendiendo cada vez más su maléfica sombra por la Tierra Media. Hombres, elfos y enanos unen sus fuerzas para presentar batalla a Sauron y sus huestes. Ajenos a estos preparativos, Frodo y Sam siguen adentrándose en el país de Mordor en su heroico viaje para destruir el Anillo de Poder en las Grietas del Destino. «Un final triunfante... un gran trabajo, tanto en la concepción como en la ejecución.» —Daily Telegraph «Un trabajo extraordinariamente imaginativo, parte saga, parte alegoría, y emocionante en su totalidad.» —The Times</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2005</t>
+          <t>2010-07-15</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Alan Lee</t>
+          <t>J. R. R. Tolkien</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>LCZvVRqH-m8C</t>
+          <t>Ndgf0AEACAAJ</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -694,46 +694,46 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1999-05</t>
+          <t>2007</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Terry Donaldson</t>
+          <t>John Ronald Reuel Tolkien</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>LvsQ34A1fOMC</t>
+          <t>PC8AAAAACAAJ</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>El Señor de los Anillos no 03/03 El Retorno del Rey (edición revisada)</t>
+          <t>El Señor de los Anillos</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>La tercera entrega de la trilogía El Señor de los Anillos. Los ejércitos del Señor Oscuro van extendiendo cada vez más su maléfica sombra por la Tierra Media. Hombres, elfos y enanos unen sus fuerzas para presentar batalla a Sauron y sus huestes. Ajenos a estos preparativos, Frodo y Sam siguen adentrándose en el país de Mordor en su heroico viaje para destruir el Anillo de Poder en las Grietas del Destino. «Un final triunfante... un gran trabajo, tanto en la concepción como en la ejecución.» —Daily Telegraph «Un trabajo extraordinariamente imaginativo, parte saga, parte alegoría, y emocionante en su totalidad.» —The Times</t>
+          <t>Ediciones Minotauro se complace en presentar la publicacion oficial y autorizada de La Comunidad del Anillo. Clbum de la pelicula, coincidiendo con el estreno de la primera parte de la trilogia epica de Peter Jackson.</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2010-07-15</t>
+          <t>2001</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>J. R. R. Tolkien</t>
+          <t>Jude Fisher</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Ndgf0AEACAAJ</t>
+          <t>QtSEvgEACAAJ</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -748,7 +748,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2007</t>
+          <t>1998</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -760,39 +760,35 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>PC8AAAAACAAJ</t>
+          <t>RYr8sgEACAAJ</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>El Señor de los Anillos</t>
+          <t>Fellowship of the Ring</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Ediciones Minotauro se complace en presentar la publicacion oficial y autorizada de La Comunidad del Anillo. Clbum de la pelicula, coincidiendo con el estreno de la primera parte de la trilogia epica de Peter Jackson.</t>
+          <t>Desconocido</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2001</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Jude Fisher</t>
-        </is>
-      </c>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>QtSEvgEACAAJ</t>
+          <t>T8P3AAAACAAJ</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>El señor de los anillos</t>
+          <t>Tolkien, el Señor de Los Anillos</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -802,47 +798,51 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>1998</t>
+          <t>2004-09-01</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>John Ronald Reuel Tolkien</t>
+          <t>J. R. R. Tolkien</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>RYr8sgEACAAJ</t>
+          <t>U7sA0AEACAAJ</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Fellowship of the Ring</t>
+          <t>El Señor de los Anillos III</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>Los ejércitos del Señor Oscuro van extendiendo cada vez más su maléfica sombra por la Tierra Media. Hombres, elfos y enanos unen sus fuerzas para presentar batalla a Sauron y sus huestes. Ajenos a estos preparativos, Frodo y Sam siguen adentrándose en el país de Mordor en su heroico viaje para destruir el Anillo de Poder en las Grietas del Destino.</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2000</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr"/>
+          <t>2010-04-28</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>John Ronald Reuel Tolkien</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>T8P3AAAACAAJ</t>
+          <t>UfYGAAAACAAJ</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Tolkien, el Señor de Los Anillos</t>
+          <t>El señor de los anillos</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -852,24 +852,24 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2004-09-01</t>
+          <t>2002-02</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>J. R. R. Tolkien</t>
+          <t>Kurt D. Bruner, Jim Ware</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>UfYGAAAACAAJ</t>
+          <t>WmdWtQAACAAJ</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>El señor de los anillos</t>
+          <t>El Señor de los anillos</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -879,24 +879,24 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2002-02</t>
+          <t>2002</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Kurt D. Bruner, Jim Ware</t>
+          <t>J. R. R. Tolkien</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>WmdWtQAACAAJ</t>
+          <t>ZVwX0QEACAAJ</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>El Señor de los anillos</t>
+          <t>El Señor de los Anillos</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -906,7 +906,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2002</t>
+          <t>1985</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -918,211 +918,211 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>ZVwX0QEACAAJ</t>
+          <t>aWZzLPhY4o0C</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>El Señor de los Anillos</t>
+          <t>The Fellowship Of The Ring</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>Begin your journey into Middle-earth... The inspiration for the upcoming original series on Prime Video, The Lord of the Rings: The Rings of Power. The Fellowship of the Ring is the first part of J.R.R. Tolkien’s epic adventure The Lord of the Rings. One Ring to rule them all, One Ring to find them, One Ring to bring them all and in the darkness bind them. Sauron, the Dark Lord, has gathered to him all the Rings of Power—the means by which he intends to rule Middle-earth. All he lacks in his plans for dominion is the One Ring—the ring that rules them all—which has fallen into the hands of the hobbit, Bilbo Baggins. In a sleepy village in the Shire, young Frodo Baggins finds himself faced with an immense task, as his elderly cousin Bilbo entrusts the Ring to his care. Frodo must leave his home and make a perilous journey across Middle-earth to the Cracks of Doom, there to destroy the Ring and foil the Dark Lord in his evil purpose.</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1985</t>
+          <t>2012-02-15</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>J. R. R. Tolkien</t>
+          <t>J.R.R. Tolkien</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>ZcAlEAAAQBAJ</t>
+          <t>ayczzwEACAAJ</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>The Lord of the Rings Illustrated</t>
+          <t>El señor de los anillos</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>A sumptuous slipcased edition of Tolkien's classic epic tale of adventure, fully illustrated in color by the author himself. This deluxe volume is quarterbound in leather and includes many special features unique to this edition. Since it was first published in 1954, The Lord of the Rings has been a book people have treasured. Steeped in unrivalled magic and otherworldliness, its sweeping fantasy and epic adventure has touched the hearts of young and old alike. Over 100 million copies of its many editions have been sold around the world, and occasional collectors' editions become prized and valuable items of publishing. This one-volume deluxe slipcased edition contains the complete text, fully corrected and reset, which is printed in red and black, and features thirty color illustrations, maps, and sketches drawn by Tolkien himself as he composed this epic work. These include the pages from the Book of Mazarbul, marvelous facsimiles created by Tolkien to accompany the famous "Bridge of Khazad-dum" chapter. Also appearing are two poster-size, fold-out maps revealing all the detail of Middle-earth. This very special deluxe edition is quarterbound in cloth and red leather, with raised ribs on the spine and stamped in two foils. The pages are edged in gold and contained within are special features unique to this edition.</t>
+          <t>Desconocido</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2021-10-19</t>
+          <t>1988</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>J. R. R. Tolkien</t>
+          <t>John Ronald Ruelen Tolkien</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>aWZzLPhY4o0C</t>
+          <t>cURzPgAACAAJ</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>The Fellowship Of The Ring</t>
+          <t>El señor de los anillos</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Begin your journey into Middle-earth... The inspiration for the upcoming original series on Prime Video, The Lord of the Rings: The Rings of Power. The Fellowship of the Ring is the first part of J.R.R. Tolkien’s epic adventure The Lord of the Rings. One Ring to rule them all, One Ring to find them, One Ring to bring them all and in the darkness bind them. Sauron, the Dark Lord, has gathered to him all the Rings of Power—the means by which he intends to rule Middle-earth. All he lacks in his plans for dominion is the One Ring—the ring that rules them all—which has fallen into the hands of the hobbit, Bilbo Baggins. In a sleepy village in the Shire, young Frodo Baggins finds himself faced with an immense task, as his elderly cousin Bilbo entrusts the Ring to his care. Frodo must leave his home and make a perilous journey across Middle-earth to the Cracks of Doom, there to destroy the Ring and foil the Dark Lord in his evil purpose.</t>
+          <t>Desconocido</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2012-02-15</t>
+          <t>1993</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>J.R.R. Tolkien</t>
+          <t>John Ronald Reuel Tolkien</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>ayczzwEACAAJ</t>
+          <t>e1ZJzwEACAAJ</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>El señor de los anillos</t>
+          <t>El Señor de Los Anillos 3. El Retorno del Rey (TV Tie-In). the Lord of the Rings 3. the Return of the King (TV Tie-In) (Spanish Edition)</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>La última parte del viaje de Frodo y Sam Los ejércitos del Señor Oscuro van extendiendo cada vez más su maléfica sombra por la Tierra Media. Hombres, elfos y enanos unen sus fuerzas para presentar batalla a Sauron y sus huestes. Ajenos a estos preparativos, Frodo y Sam siguen adentrándose en el país de Mordor en su heroico viaje para destruir el Anillo de Poder en las Grietas del Destino. ENGLISH DESCRIPTION The Return of the King is the third part of J.R.R. Tolkien's epic adventure The Lord of the Rings. One Ring to rule them all, One Ring to find them, One Ring to bring them all and in the darkness bind them. The Dark Lord has risen, and as he unleashes hordes of Orcs to conquer all Middle-earth, Frodo and Sam struggle deep into his realm in Mordor. To defeat Sauron, the One Ring must be destroyed in the fires of Mount Doom. But the way is impossibly hard, and Frodo is weakening. The Ring corrupts all who bear it and Frodo's time is running out. Will Sam and Frodo succeed, or will the Dark Lord rule Middle-earth once more?</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1988</t>
+          <t>2022-09-27</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>John Ronald Ruelen Tolkien</t>
+          <t>J. R. R. Tolkien</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>cURzPgAACAAJ</t>
+          <t>eVQGEQAAQBAJ</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>El señor de los anillos</t>
+          <t>The Worm Ouroboros</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>"The Worm Ouroboros" by Eric Rücker Eddison is a classic fantasy novel that transports readers to the enchanting world of Mercury, where two rival kingdoms, Witchland and Demonland, engage in a timeless struggle for power and supremacy. Set against a backdrop of epic battles, intricate political intrigues, and mythical creatures, the novel follows the adventures of heroes and villains alike as they navigate a landscape fraught with magic and danger. Eddison's rich prose and vivid imagination create a captivating tale that explores themes of honor, loyalty, and the eternal conflict between good and evil. A timeless masterpiece of fantasy literature, "The Worm Ouroboros" continues to enchant readers with its immersive world-building and compelling storytelling.</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1993</t>
+          <t>2024-05-07</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>John Ronald Reuel Tolkien</t>
+          <t>Eric Rücker Eddison</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>e1ZJzwEACAAJ</t>
+          <t>gHzeCYjKGBsC</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>El Señor de Los Anillos 3. El Retorno del Rey (TV Tie-In). the Lord of the Rings 3. the Return of the King (TV Tie-In) (Spanish Edition)</t>
+          <t>El señor de los anillos y la filosofía</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>La última parte del viaje de Frodo y Sam Los ejércitos del Señor Oscuro van extendiendo cada vez más su maléfica sombra por la Tierra Media. Hombres, elfos y enanos unen sus fuerzas para presentar batalla a Sauron y sus huestes. Ajenos a estos preparativos, Frodo y Sam siguen adentrándose en el país de Mordor en su heroico viaje para destruir el Anillo de Poder en las Grietas del Destino. ENGLISH DESCRIPTION The Return of the King is the third part of J.R.R. Tolkien's epic adventure The Lord of the Rings. One Ring to rule them all, One Ring to find them, One Ring to bring them all and in the darkness bind them. The Dark Lord has risen, and as he unleashes hordes of Orcs to conquer all Middle-earth, Frodo and Sam struggle deep into his realm in Mordor. To defeat Sauron, the One Ring must be destroyed in the fires of Mount Doom. But the way is impossibly hard, and Frodo is weakening. The Ring corrupts all who bear it and Frodo's time is running out. Will Sam and Frodo succeed, or will the Dark Lord rule Middle-earth once more?</t>
+          <t>¿Nos resultaría aburrida la vida eterna en caso de que pudiéramos alcanzarla? ¿Qué virtudes son necesarias para que el poder no corrompa a quien lo tiene? ¿Se revelará la naturaleza contra la tecnología? Si un ente cae en el bosque y nadie lo oye, ¿hace ruido? Gregory Bassham y Eric Bronson dan respuesta a éstas y otras cuestiones planteadas en El Señor de los Anillos, la epopeya de J. R. R. Tolkien que, desde su publicación, ha vendido más de cincuenta millones de ejemplares y cuya riqueza y complejidad ha tejido una red cada vez más amplia de seguidores. Si la intención de Tolkien era crear «una historia que mantendría la atención del lector [...] y que a veces quizá lo excitaría o lo conmovería profundamente», consiguió también trasladar a su obra algunas de sus propias inquietudes filosóficas: la lucha del bien contra el mal, la oposición entre destino y libre albedrío, la búsqueda de la felicidad o la vida después de la muerte. Esta colección de ensayos además de ofrecernos una comprensión más fiel de las cuestiones que inspiran y nutren El Señor de los Anillos, supone una amena introducción a la filosofía, la religión y la mitología y una excelente carta de presentación a la cosmovisión de pensadores como Platón, Aristóteles o Nietzsche. Porque, como dice el mago filósofo Gandalf: "Si has estado estos días con las orejas tapadas y la mente dormida, ¡es hora de que despiertes!</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2022-09-27</t>
+          <t>2010-05-20</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>J. R. R. Tolkien</t>
+          <t>Gregory Bassham, Eric Bronson</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>gHzeCYjKGBsC</t>
+          <t>jZgjyAEACAAJ</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>El señor de los anillos y la filosofía</t>
+          <t>The Return of the King</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>¿Nos resultaría aburrida la vida eterna en caso de que pudiéramos alcanzarla? ¿Qué virtudes son necesarias para que el poder no corrompa a quien lo tiene? ¿Se revelará la naturaleza contra la tecnología? Si un ente cae en el bosque y nadie lo oye, ¿hace ruido? Gregory Bassham y Eric Bronson dan respuesta a éstas y otras cuestiones planteadas en El Señor de los Anillos, la epopeya de J. R. R. Tolkien que, desde su publicación, ha vendido más de cincuenta millones de ejemplares y cuya riqueza y complejidad ha tejido una red cada vez más amplia de seguidores. Si la intención de Tolkien era crear «una historia que mantendría la atención del lector [...] y que a veces quizá lo excitaría o lo conmovería profundamente», consiguió también trasladar a su obra algunas de sus propias inquietudes filosóficas: la lucha del bien contra el mal, la oposición entre destino y libre albedrío, la búsqueda de la felicidad o la vida después de la muerte. Esta colección de ensayos además de ofrecernos una comprensión más fiel de las cuestiones que inspiran y nutren El Señor de los Anillos, supone una amena introducción a la filosofía, la religión y la mitología y una excelente carta de presentación a la cosmovisión de pensadores como Platón, Aristóteles o Nietzsche. Porque, como dice el mago filósofo Gandalf: "Si has estado estos días con las orejas tapadas y la mente dormida, ¡es hora de que despiertes!</t>
+          <t>Desconocido</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2010-05-20</t>
+          <t>1967</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Gregory Bassham, Eric Bronson</t>
+          <t>John Ronald Reuel Tolkien</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>jZgjyAEACAAJ</t>
+          <t>ld5GswEACAAJ</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>The Return of the King</t>
+          <t>The Fellowship of the Ring</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>Frodo the hobbit and a band of warriors from the different kingdoms set out to destroy the Ring of Power before the evil Sauron grasps control.</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>1967</t>
+          <t>2005</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1134,22 +1134,22 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>ld5GswEACAAJ</t>
+          <t>neSkMQEACAAJ</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>The Fellowship of the Ring</t>
+          <t>El Señor de Los Anillos 1.</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Frodo the hobbit and a band of warriors from the different kingdoms set out to destroy the Ring of Power before the evil Sauron grasps control.</t>
+          <t>La Compania se ha disuelto y sus integrantes emprenden caminos separados. Frodo y Sam continuan solos su viaje a lo largo del rio Anduin, perseguidos por la sombra misteriosa de un ser extrano que tambien ambiciona la posesion del Anillo. Mientras, hombres, elfos y enanos se preparan para la batalla final contra las fuerzas del Senor del Mal.</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2005</t>
+          <t>2012-11-13</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1161,44 +1161,44 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>neSkMQEACAAJ</t>
+          <t>o5WfPwAACAAJ</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>El Señor de Los Anillos 1.</t>
+          <t>El Señor de los anillos</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>La Compania se ha disuelto y sus integrantes emprenden caminos separados. Frodo y Sam continuan solos su viaje a lo largo del rio Anduin, perseguidos por la sombra misteriosa de un ser extrano que tambien ambiciona la posesion del Anillo. Mientras, hombres, elfos y enanos se preparan para la batalla final contra las fuerzas del Senor del Mal.</t>
+          <t>Desconocido</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2012-11-13</t>
+          <t>2002</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>John Ronald Reuel Tolkien</t>
+          <t>J. R. R. Tolkien</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>o5WfPwAACAAJ</t>
+          <t>q0JyPwAACAAJ</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>El Señor de los anillos</t>
+          <t>El Señor de Los Anillos, I</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>En la adormecida e idílica Comarca, un joven hobbit recibe un encargo: custodiar el Anillo Único y emprender el viaje para su destrucción en las Grietas del Destino. Acompañado por magos, hombres, elfos y enanos, atravesará la Tierra Media y se internará en las sombras de Mordor, perseguido siempre por las huestes de Sauron, el Señor Oscuro, dispuesto a recuperar su creación para establecer el dominio definitivo del Mal.</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1215,27 +1215,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>q0JyPwAACAAJ</t>
+          <t>sA3CAAAACAAJ</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>El Señor de Los Anillos, I</t>
+          <t>El Senor De Los Anillos Iii</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>En la adormecida e idílica Comarca, un joven hobbit recibe un encargo: custodiar el Anillo Único y emprender el viaje para su destrucción en las Grietas del Destino. Acompañado por magos, hombres, elfos y enanos, atravesará la Tierra Media y se internará en las sombras de Mordor, perseguido siempre por las huestes de Sauron, el Señor Oscuro, dispuesto a recuperar su creación para establecer el dominio definitivo del Mal.</t>
+          <t>Desconocido</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2002</t>
+          <t>2004-06-30</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>J. R. R. Tolkien</t>
+          <t>John Ronald Reuel Tolkien</t>
         </is>
       </c>
     </row>

</xml_diff>